<commit_message>
draft repartition of tasks
</commit_message>
<xml_diff>
--- a/Planning Tasks.xlsx
+++ b/Planning Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stellanwea/Documents/DE/Solidity/HW5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5705BE0-618F-E54C-932F-90DF0C63D83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7755B3F5-24AB-5448-B97E-D8CBAD1A4254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2080" yWindow="2800" windowWidth="26340" windowHeight="13960" xr2:uid="{21A3FDC3-E97C-4A45-9173-1F9893139FEA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Calida</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>GOUVERNANCE TEAM</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>fff</t>
   </si>
 </sst>
 </file>
@@ -359,43 +365,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -410,62 +389,85 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -802,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B57B3AB-4086-A84F-BCCE-E9AD96840E44}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -817,195 +819,198 @@
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="41" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="34"/>
-    </row>
-    <row r="3" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14" t="s">
+    <row r="2" spans="1:12" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="41"/>
+    </row>
+    <row r="3" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14" t="s">
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="37"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14" t="s">
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="37"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14" t="s">
+    <row r="6" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="37"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14" t="s">
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="37"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="15"/>
-    </row>
-    <row r="8" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14" t="s">
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="37"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14" t="s">
+    <row r="9" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="37"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="15"/>
-    </row>
-    <row r="10" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14" t="s">
+      <c r="I9" s="6"/>
+      <c r="L9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="37"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14" t="s">
+    <row r="11" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="37"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="15"/>
-    </row>
-    <row r="12" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="16" t="s">
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="37"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="19" t="s">
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1016,7 +1021,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1027,137 +1032,139 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
+    <row r="15" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="34" t="s">
+      <c r="H15" s="41" t="s">
         <v>31</v>
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="34"/>
+    <row r="16" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="41"/>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="14" t="s">
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="H17" s="15"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="14" t="s">
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="H18" s="15"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="14" t="s">
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="H19" s="15"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="H20" s="15"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="H20" s="6"/>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="H21" s="15"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="H21" s="6"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="1"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="H23" s="15"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="H23" s="6"/>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="19"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="10"/>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
@@ -1165,109 +1172,109 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="21" t="s">
+      <c r="B27" s="27"/>
+      <c r="C27" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="30" t="s">
+      <c r="F27" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G27" s="30" t="s">
+      <c r="G27" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="32" t="s">
+      <c r="H27" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="I27" s="34" t="s">
+      <c r="I27" s="41" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="40"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="34"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="41"/>
     </row>
     <row r="29" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="40"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="24" t="s">
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="35"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="17"/>
     </row>
     <row r="30" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="40"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="14" t="s">
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="36"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="18"/>
     </row>
     <row r="31" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="40"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="36"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="18"/>
     </row>
     <row r="32" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="40"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="36"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="18"/>
     </row>
     <row r="33" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="42"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="37"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="19"/>
     </row>
     <row r="34" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
@@ -1295,22 +1302,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="A27:B33"/>
-    <mergeCell ref="A15:B24"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="A1:B12"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="C15:C16"/>
     <mergeCell ref="H27:H28"/>
     <mergeCell ref="H15:H16"/>
     <mergeCell ref="C1:C2"/>
@@ -1318,6 +1309,22 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="A1:B12"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A27:B33"/>
+    <mergeCell ref="A15:B24"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update token team planning
</commit_message>
<xml_diff>
--- a/Planning Tasks.xlsx
+++ b/Planning Tasks.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stellanwea/Documents/DE/Solidity/HW5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hortensevallat/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7755B3F5-24AB-5448-B97E-D8CBAD1A4254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D3D354-3D78-1C41-8E1D-604F3D8ECB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="2800" windowWidth="26340" windowHeight="13960" xr2:uid="{21A3FDC3-E97C-4A45-9173-1F9893139FEA}"/>
+    <workbookView xWindow="2080" yWindow="2640" windowWidth="26340" windowHeight="13960" xr2:uid="{21A3FDC3-E97C-4A45-9173-1F9893139FEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>Calida</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Propose ideas of token</t>
   </si>
   <si>
-    <t>Implement through code this code</t>
-  </si>
-  <si>
     <t>Design a voting system</t>
   </si>
   <si>
@@ -137,10 +134,16 @@
     <t>GOUVERNANCE TEAM</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>fff</t>
+    <t>Adding comments on the code</t>
+  </si>
+  <si>
+    <t>Adding functions to get token rewards</t>
+  </si>
+  <si>
+    <t>Making final checks with the governance team</t>
+  </si>
+  <si>
+    <t>Implement through code this token</t>
   </si>
 </sst>
 </file>
@@ -365,13 +368,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -404,24 +406,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -443,32 +472,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -804,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B57B3AB-4086-A84F-BCCE-E9AD96840E44}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -819,15 +827,15 @@
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="20" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="24" t="s">
@@ -839,178 +847,175 @@
       <c r="G1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="23"/>
+      <c r="I1" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="41"/>
-    </row>
-    <row r="3" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="37"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="5" t="s">
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
+    </row>
+    <row r="3" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="37"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="5" t="s">
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="30"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="5" t="s">
+      <c r="I5" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="30"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="30"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="5" t="s">
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="30"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="37"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>30</v>
+      <c r="I8" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="30"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="6"/>
-      <c r="L9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="37"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="5" t="s">
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="30"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="3"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="5" t="s">
+      <c r="I10" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="37"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="7" t="s">
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="30"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1021,7 +1026,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1032,129 +1037,151 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="32" t="s">
+    <row r="15" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="20" t="s">
+      <c r="B15" s="40"/>
+      <c r="C15" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="41" t="s">
-        <v>31</v>
+      <c r="H15" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="41"/>
+    <row r="16" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="21"/>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="5" t="s">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="H17" s="6"/>
+      <c r="G17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="5"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="5" t="s">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="4"/>
+      <c r="D18" s="3"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="H18" s="6"/>
+      <c r="G18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="5"/>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="H19" s="6"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="41"/>
+      <c r="H19" s="5"/>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="4"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="H20" s="6"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="5"/>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="32"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="4"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="H21" s="6"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="5"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="32"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="4"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="3"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="G22" s="41"/>
+      <c r="H22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="32"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="4"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="3"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="H23" s="6"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="5"/>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="32"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="10"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="9"/>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1180,14 +1207,14 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="20" t="s">
+      <c r="A27" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="35"/>
+      <c r="C27" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="32" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="24" t="s">
@@ -1199,82 +1226,82 @@
       <c r="G27" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="39" t="s">
+      <c r="H27" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I27" s="41" t="s">
-        <v>31</v>
+      <c r="I27" s="21" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="28"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="23"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="33"/>
       <c r="E28" s="25"/>
       <c r="F28" s="25"/>
       <c r="G28" s="25"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="41"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="21"/>
     </row>
     <row r="29" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="28"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="11" t="s">
+      <c r="A29" s="36"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="16"/>
+    </row>
+    <row r="30" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="36"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="17"/>
-    </row>
-    <row r="30" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="28"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="18"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="28"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="5"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="4"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="18"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="17"/>
     </row>
     <row r="32" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="28"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="5"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="4"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="18"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="17"/>
     </row>
     <row r="33" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="30"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="19"/>
+      <c r="A33" s="38"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="18"/>
     </row>
     <row r="34" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
@@ -1302,19 +1329,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="A1:B12"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="C15:C16"/>
     <mergeCell ref="A27:B33"/>
     <mergeCell ref="A15:B24"/>
     <mergeCell ref="D15:D16"/>
@@ -1324,6 +1338,19 @@
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="E27:E28"/>
     <mergeCell ref="F27:F28"/>
+    <mergeCell ref="A1:B12"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="G15:G16"/>
     <mergeCell ref="G27:G28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>